<commit_message>
fix wr crn off bugs by Shaojian at 11:00 am 9.17
</commit_message>
<xml_diff>
--- a/input_sample/M18104948C/M18104948C_crn_stk.xlsx
+++ b/input_sample/M18104948C/M18104948C_crn_stk.xlsx
@@ -112,7 +112,7 @@
     <t>-0.0658</t>
   </si>
   <si>
-    <t>-0.0566</t>
+    <t>-0.1766</t>
   </si>
   <si>
     <t>-0.0000</t>
@@ -214,10 +214,10 @@
     <t>-0.0300</t>
   </si>
   <si>
-    <t>-0.4006</t>
-  </si>
-  <si>
-    <t>-0.3504</t>
+    <t>-0.6006</t>
+  </si>
+  <si>
+    <t>-0.5504</t>
   </si>
   <si>
     <t>-0.0503</t>

</xml_diff>

<commit_message>
fix Ef_En_PU_Prf3 func call bug in penv
</commit_message>
<xml_diff>
--- a/input_sample/M18104948C/M18104948C_crn_stk.xlsx
+++ b/input_sample/M18104948C/M18104948C_crn_stk.xlsx
@@ -214,10 +214,10 @@
     <t>-0.0300</t>
   </si>
   <si>
-    <t>-0.6006</t>
-  </si>
-  <si>
-    <t>-0.5504</t>
+    <t>-0.1006</t>
+  </si>
+  <si>
+    <t>-0.1504</t>
   </si>
   <si>
     <t>-0.0503</t>

</xml_diff>